<commit_message>
RolePermission for all view
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nnquynh-laptop\source\repos\ICMSsolution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9983F70-4632-4DE8-B4B2-DF8FA9DAD5E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB61819-F9BB-4F2D-8CAE-F22197EF09DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="748" activeTab="9" xr2:uid="{919F9413-3E8B-4FC3-9CC5-F2E101C40464}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="748" activeTab="5" xr2:uid="{919F9413-3E8B-4FC3-9CC5-F2E101C40464}"/>
   </bookViews>
   <sheets>
     <sheet name="City" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,11 @@
     <sheet name="User" sheetId="12" r:id="rId10"/>
     <sheet name="UserDefault" sheetId="20" r:id="rId11"/>
     <sheet name="PermissionFunc" sheetId="21" r:id="rId12"/>
-    <sheet name="RolePermission" sheetId="22" r:id="rId13"/>
-    <sheet name="Customer" sheetId="13" r:id="rId14"/>
-    <sheet name="Machine" sheetId="15" r:id="rId15"/>
-    <sheet name="Sensor" sheetId="16" r:id="rId16"/>
-    <sheet name="Certificate" sheetId="18" r:id="rId17"/>
-    <sheet name="CalibData" sheetId="17" r:id="rId18"/>
+    <sheet name="Customer" sheetId="13" r:id="rId13"/>
+    <sheet name="Machine" sheetId="15" r:id="rId14"/>
+    <sheet name="Sensor" sheetId="16" r:id="rId15"/>
+    <sheet name="Certificate" sheetId="18" r:id="rId16"/>
+    <sheet name="CalibData" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -87,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="663" uniqueCount="552">
   <si>
     <t>An Giang</t>
   </si>
@@ -1692,9 +1691,6 @@
   </si>
   <si>
     <t>Loại đầu dò</t>
-  </si>
-  <si>
-    <t>PermissionFuncId</t>
   </si>
   <si>
     <t>Permission</t>
@@ -3598,9 +3594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E163219-7505-435D-893C-049CC5135536}">
   <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,7 +3667,7 @@
         <v>92</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D3" s="26">
         <v>4</v>
@@ -3707,7 +3703,7 @@
         <v>91</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D4" s="26">
         <v>3</v>
@@ -3743,7 +3739,7 @@
         <v>93</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D5" s="26">
         <v>3</v>
@@ -3815,7 +3811,7 @@
         <v>482</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -3851,7 +3847,7 @@
         <v>490</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -3887,7 +3883,7 @@
         <v>484</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -3923,7 +3919,7 @@
         <v>486</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -3959,7 +3955,7 @@
         <v>488</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -4478,36 +4474,6 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2E7BF16-DBF4-444F-81E6-F2FB48FC2F6B}">
-  <dimension ref="B1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="3" max="3" width="17.140625" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" t="s">
-        <v>535</v>
-      </c>
-      <c r="D1" t="s">
-        <v>536</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C2640C8-9A74-45B1-90FD-1832E1F5DC3C}">
   <dimension ref="A1:W545"/>
   <sheetViews>
@@ -6287,7 +6253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FF4C8B-CB6E-4BC6-8C73-CA20681E2A27}">
   <dimension ref="A1:W5"/>
   <sheetViews>
@@ -6489,7 +6455,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EBB7903-0DF5-443B-A373-721E477368B3}">
   <dimension ref="A1:V5"/>
   <sheetViews>
@@ -6677,7 +6643,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66025D19-6A72-4222-9D26-7C00155F1A8B}">
   <dimension ref="A1:AB14"/>
   <sheetViews>
@@ -6961,7 +6927,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26A97B93-E3C6-48E4-95D2-5FE9FD5F0FAD}">
   <dimension ref="A1:Z5"/>
   <sheetViews>
@@ -8801,8 +8767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE37355-416D-442C-B59D-AE8761DFDD82}">
   <dimension ref="A1:AJ48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:AJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8832,13 +8798,13 @@
         <v>513</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>536</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>537</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>538</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>510</v>
@@ -9001,7 +8967,7 @@
       </c>
       <c r="L3" s="3">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M3" s="3">
         <f t="shared" si="1"/>
@@ -9017,7 +8983,7 @@
       </c>
       <c r="Q3" s="45" t="str">
         <f t="shared" ref="Q3:Q6" si="2">_xlfn.CONCAT("if not exists (SELECT * FROM  dbo.Role where [Name] = N'",A3,"') BEGIN INSERT INTO dbo.Role  ([Name], [User], [Permission],[BackupDB], [RestoreDB],[RadQuantity],[DoseQuantity],[Unit],[TM],[Certificate],[Customer],[City],[MachineName],[MachineType],[SensorType]) VALUES (N'",A3,"', ",B3,", ",C3,", ",D3,", ",E3,", ",F3,", ",G3,", ",H3,", ",I3,", ",J3,", ",K3,", ",L3,", ",M3,", ",N3,", ",O3,"); END")</f>
-        <v>if not exists (SELECT * FROM  dbo.Role where [Name] = N'Technical') BEGIN INSERT INTO dbo.Role  ([Name], [User], [Permission],[BackupDB], [RestoreDB],[RadQuantity],[DoseQuantity],[Unit],[TM],[Certificate],[Customer],[City],[MachineName],[MachineType],[SensorType]) VALUES (N'Technical', 0, 0, 0, 0, 16, 16, 16, 28, 31, 28, 16, 30, 28, 28); END</v>
+        <v>if not exists (SELECT * FROM  dbo.Role where [Name] = N'Technical') BEGIN INSERT INTO dbo.Role  ([Name], [User], [Permission],[BackupDB], [RestoreDB],[RadQuantity],[DoseQuantity],[Unit],[TM],[Certificate],[Customer],[City],[MachineName],[MachineType],[SensorType]) VALUES (N'Technical', 0, 0, 0, 0, 16, 16, 16, 28, 31, 28, 28, 30, 28, 28); END</v>
       </c>
       <c r="R3" s="45"/>
       <c r="S3" s="45"/>
@@ -9355,7 +9321,7 @@
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B11" s="39">
         <v>1</v>
@@ -9402,7 +9368,7 @@
     </row>
     <row r="12" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A12" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B12" s="28">
         <v>0</v>
@@ -9447,7 +9413,7 @@
     </row>
     <row r="13" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A13" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B13" s="28">
         <v>0</v>
@@ -9494,7 +9460,7 @@
     </row>
     <row r="14" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A14" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B14" s="28">
         <v>0</v>
@@ -9539,7 +9505,7 @@
     </row>
     <row r="15" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A15" s="34" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B15" s="28"/>
       <c r="C15" s="28"/>
@@ -9560,7 +9526,7 @@
     </row>
     <row r="16" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B16" s="43">
         <f>B15+B14*2+B13*2^2+B12*2^3+B11*2^4</f>
@@ -9694,7 +9660,7 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B19" s="39">
         <v>0</v>
@@ -9741,7 +9707,7 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B20" s="28">
         <v>0</v>
@@ -9772,7 +9738,7 @@
         <v>1</v>
       </c>
       <c r="L20" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M20" s="28">
         <v>1</v>
@@ -9786,7 +9752,7 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B21" s="28">
         <v>0</v>
@@ -9819,7 +9785,7 @@
         <v>1</v>
       </c>
       <c r="L21" s="28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M21" s="28">
         <v>1</v>
@@ -9833,7 +9799,7 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B22" s="28">
         <v>0</v>
@@ -9878,7 +9844,7 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="34" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
@@ -9899,7 +9865,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B24" s="43">
         <f>B23+B22*2+B21*2^2+B20*2^3+B19*2^4</f>
@@ -9943,7 +9909,7 @@
       </c>
       <c r="L24" s="43">
         <f t="shared" ref="L24" si="28">L23+L22*2+L21*2^2+L20*2^3+L19*2^4</f>
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="M24" s="43">
         <f t="shared" ref="M24" si="29">M23+M22*2+M21*2^2+M20*2^3+M19*2^4</f>
@@ -10033,7 +9999,7 @@
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B27" s="39">
         <v>1</v>
@@ -10080,7 +10046,7 @@
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B28" s="28">
         <v>1</v>
@@ -10125,7 +10091,7 @@
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B29" s="28">
         <v>1</v>
@@ -10172,7 +10138,7 @@
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B30" s="28">
         <v>0</v>
@@ -10217,7 +10183,7 @@
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="34" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
@@ -10238,7 +10204,7 @@
     </row>
     <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B32" s="43">
         <f>B31+B30*2+B29*2^2+B28*2^3+B27*2^4</f>
@@ -10361,7 +10327,7 @@
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B35" s="39">
         <v>1</v>
@@ -10408,7 +10374,7 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B36" s="28">
         <v>1</v>
@@ -10453,7 +10419,7 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B37" s="28">
         <v>1</v>
@@ -10500,7 +10466,7 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B38" s="28">
         <v>1</v>
@@ -10545,7 +10511,7 @@
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="34" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B39" s="29"/>
       <c r="C39" s="29"/>
@@ -10566,7 +10532,7 @@
     </row>
     <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B40" s="43">
         <f>B39+B38*2+B37*2^2+B36*2^3+B35*2^4</f>
@@ -10689,7 +10655,7 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B43" s="39">
         <v>1</v>
@@ -10736,7 +10702,7 @@
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="33" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B44" s="28">
         <v>1</v>
@@ -10781,7 +10747,7 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="B45" s="28">
         <v>1</v>
@@ -10828,7 +10794,7 @@
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B46" s="44">
         <v>1</v>
@@ -10873,7 +10839,7 @@
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="34" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B47" s="29"/>
       <c r="C47" s="29"/>
@@ -10894,7 +10860,7 @@
     </row>
     <row r="48" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="35" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B48" s="43">
         <f>B47+B46*2+B45*2^2+B44*2^3+B43*2^4</f>

</xml_diff>